<commit_message>
update excel file for muni debt commentary
</commit_message>
<xml_diff>
--- a/output/commentary_muni_debt_ranking.xlsx
+++ b/output/commentary_muni_debt_ranking.xlsx
@@ -1061,19 +1061,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>prince william county public schools</t>
+          <t>rutherford county schools</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="D2">
-        <v>-647518149</v>
+        <v>-76790573</v>
       </c>
       <c r="E2">
-        <v>-7189.054613078716</v>
+        <v>-1559.104480945323</v>
       </c>
     </row>
     <row r="3">
@@ -1091,10 +1091,10 @@
         </is>
       </c>
       <c r="D3">
-        <v>-131942140</v>
+        <v>-65971070</v>
       </c>
       <c r="E3">
-        <v>-1771.36831082351</v>
+        <v>-885.6841554117552</v>
       </c>
     </row>
     <row r="4">
@@ -1166,12 +1166,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>baltimore city public school system</t>
+          <t>detroit public schools</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="D7">
@@ -1187,12 +1187,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>detroit public schools</t>
+          <t>hawaii department of education</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Hawaii</t>
         </is>
       </c>
       <c r="D8">
@@ -1208,19 +1208,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>hawaii department of education</t>
+          <t>board of education of baltimore county</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hawaii</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1844637</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>16.59801504463</v>
       </c>
     </row>
     <row r="10">
@@ -1229,19 +1229,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>board of education of baltimore county</t>
+          <t>chesterfield county school board</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="D10">
-        <v>1844637</v>
+        <v>4167372</v>
       </c>
       <c r="E10">
-        <v>16.59801504463</v>
+        <v>66.73668027864521</v>
       </c>
     </row>
     <row r="11">
@@ -1250,19 +1250,19 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>chesterfield county school board</t>
+          <t>city and county of denver school district no. 1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="D11">
-        <v>4167372</v>
+        <v>30587841</v>
       </c>
       <c r="E11">
-        <v>66.73668027864521</v>
+        <v>344.027634375949</v>
       </c>
     </row>
   </sheetData>
@@ -1659,145 +1659,145 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>philadelphia</t>
+          <t>austin</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C4">
-        <v>7543068000</v>
+        <v>6277143000</v>
       </c>
       <c r="D4">
-        <v>4703.250220258275</v>
+        <v>6525.775028589251</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>austin</t>
+          <t>phoenix</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="C5">
-        <v>6277143000</v>
+        <v>4744660000</v>
       </c>
       <c r="D5">
-        <v>6525.775028589251</v>
+        <v>2950.31059762839</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>phoenix</t>
+          <t>houston</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C6">
-        <v>4744660000</v>
+        <v>4542769000</v>
       </c>
       <c r="D6">
-        <v>2950.31059762839</v>
+        <v>1973.767929050232</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>houston</t>
+          <t>portland</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="C7">
-        <v>4542769000</v>
+        <v>4381080492</v>
       </c>
       <c r="D7">
-        <v>1973.767929050232</v>
+        <v>6714.114387649076</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>portland</t>
+          <t>boston</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="C8">
-        <v>4381080492</v>
+        <v>3390433000</v>
       </c>
       <c r="D8">
-        <v>6714.114387649076</v>
+        <v>5018.165214199445</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>boston</t>
+          <t>jacksonville</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="C9">
-        <v>3390433000</v>
+        <v>3244209000</v>
       </c>
       <c r="D9">
-        <v>5018.165214199445</v>
+        <v>3416.337761790029</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>jacksonville</t>
+          <t>san jose</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>California</t>
         </is>
       </c>
       <c r="C10">
-        <v>3244209000</v>
+        <v>3116478000</v>
       </c>
       <c r="D10">
-        <v>3416.337761790029</v>
+        <v>3075.812680550443</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>san jose</t>
+          <t>fort worth</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C11">
-        <v>3116478000</v>
+        <v>2926444000</v>
       </c>
       <c r="D11">
-        <v>3075.812680550443</v>
+        <v>3184.596985429904</v>
       </c>
     </row>
   </sheetData>
@@ -2000,19 +2000,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>philadelphia</t>
+          <t>miami</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="C11">
-        <v>4703.250220258275</v>
+        <v>4700.251071767739</v>
       </c>
       <c r="D11">
-        <v>7543068000</v>
+        <v>2078733039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
taking jacksonville out of city list
</commit_message>
<xml_diff>
--- a/output/commentary_muni_debt_ranking.xlsx
+++ b/output/commentary_muni_debt_ranking.xlsx
@@ -522,7 +522,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -531,238 +531,203 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>state.name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>state.name</t>
+          <t>total_pension_liability</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>total_pension_liability</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>total_pension_liability_pc</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>2022</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>chicago board of education</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>chicago board of education</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>Illinois</t>
         </is>
       </c>
+      <c r="C2">
+        <v>18032391000</v>
+      </c>
       <c r="D2">
-        <v>18032391000</v>
-      </c>
-      <c r="E2">
         <v>54670.77881128804</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>2022</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>los angeles unified school district</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>los angeles unified school district</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>California</t>
         </is>
       </c>
+      <c r="C3">
+        <v>14497900000</v>
+      </c>
       <c r="D3">
-        <v>14497900000</v>
-      </c>
-      <c r="E3">
         <v>33255.26770927475</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>2022</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>school district of philadelphia</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>school district of philadelphia</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>Pennsylvania</t>
         </is>
       </c>
+      <c r="C4">
+        <v>3461400000</v>
+      </c>
       <c r="D4">
-        <v>3461400000</v>
-      </c>
-      <c r="E4">
         <v>29320.72882518869</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>2022</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>the board of education of montgomery county</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>new york city geographic district # 31</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
+          <t>Maryland</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>2927620795</v>
       </c>
       <c r="D5">
-        <v>3081147150.07085</v>
-      </c>
-      <c r="E5">
-        <v>50719.3064918081</v>
+        <v>18502.19486067837</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>2022</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>prince george’s county public schools</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>the board of education of montgomery county</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>Maryland</t>
         </is>
       </c>
+      <c r="C6">
+        <v>2741734238</v>
+      </c>
       <c r="D6">
-        <v>2927620795</v>
-      </c>
-      <c r="E6">
-        <v>18502.19486067837</v>
+        <v>21291.71575677565</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>2022</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>fairfax county public schools</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>new york city geographic district # 2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>2543975359</v>
       </c>
       <c r="D7">
-        <v>2885573504.238444</v>
-      </c>
-      <c r="E7">
-        <v>50719.3064918082</v>
+        <v>14253.63969430577</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>2022</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>clark county school district</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>prince george’s county public schools</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
+          <t>Nevada</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>2542613302</v>
+      </c>
+      <c r="D8">
+        <v>8051.671861096245</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>wake county board of education</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>2120234842</v>
+      </c>
+      <c r="D9">
+        <v>13243.2734870299</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>charlotte-mecklenburg board of education</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>1965975000</v>
+      </c>
+      <c r="D10">
+        <v>13724.658624445</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>board of education of baltimore county</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Maryland</t>
         </is>
       </c>
-      <c r="D8">
-        <v>2741734238</v>
-      </c>
-      <c r="E8">
-        <v>21291.71575677565</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>2022</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>new york city geographic district # 24</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>2631216182.182026</v>
-      </c>
-      <c r="E9">
-        <v>50719.3064918082</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>2022</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>fairfax county public schools</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Virginia</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>2543975359</v>
-      </c>
-      <c r="E10">
-        <v>14253.63969430577</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>2022</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>clark county school district</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Nevada</t>
-        </is>
+      <c r="C11">
+        <v>1844637000</v>
       </c>
       <c r="D11">
-        <v>2542613302</v>
-      </c>
-      <c r="E11">
-        <v>8051.671861096245</v>
+        <v>16598.01504463</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +737,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -781,238 +746,203 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>state.name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>state.name</t>
+          <t>total_pension_liability_pc</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>total_pension_liability_pc</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>total_pension_liability</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>2022</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>chicago board of education</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>chicago board of education</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>Illinois</t>
         </is>
       </c>
+      <c r="C2">
+        <v>54670.77881128804</v>
+      </c>
       <c r="D2">
-        <v>54670.77881128804</v>
-      </c>
-      <c r="E2">
         <v>18032391000</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>2022</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>los angeles unified school district</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>new york city geographic district # 2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>33255.26770927475</v>
       </c>
       <c r="D3">
-        <v>50719.3064918082</v>
-      </c>
-      <c r="E3">
-        <v>2885573504.238444</v>
+        <v>14497900000</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>2022</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>school district of philadelphia</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>new york city geographic district # 24</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
+          <t>Pennsylvania</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>29320.72882518869</v>
       </c>
       <c r="D4">
-        <v>50719.3064918082</v>
-      </c>
-      <c r="E4">
-        <v>2631216182.182026</v>
+        <v>3461400000</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>2022</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>prince george’s county public schools</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>new york city geographic district # 20</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
+          <t>Maryland</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>21291.71575677565</v>
       </c>
       <c r="D5">
-        <v>50719.3064918081</v>
-      </c>
-      <c r="E5">
-        <v>2408812023.215442</v>
+        <v>2741734238</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>2022</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>the board of education of montgomery county</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>new york city geographic district # 31</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
+          <t>Maryland</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>18502.19486067837</v>
       </c>
       <c r="D6">
-        <v>50719.3064918081</v>
-      </c>
-      <c r="E6">
-        <v>3081147150.07085</v>
+        <v>2927620795</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>2022</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>board of education of baltimore county</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>new york city geographic district # 10</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
+          <t>Maryland</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>16598.01504463</v>
       </c>
       <c r="D7">
-        <v>50719.30649180806</v>
-      </c>
-      <c r="E7">
-        <v>2359715734.53137</v>
+        <v>1844637000</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>2022</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fairfax county public schools</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>boston public schools</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Massachusetts</t>
-        </is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>14253.63969430577</v>
       </c>
       <c r="D8">
-        <v>40389.39873075007</v>
-      </c>
-      <c r="E8">
-        <v>1864738150</v>
+        <v>2543975359</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>2022</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>charlotte-mecklenburg board of education</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>los angeles unified school district</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>California</t>
-        </is>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>13724.658624445</v>
       </c>
       <c r="D9">
-        <v>33255.26770927475</v>
-      </c>
-      <c r="E9">
-        <v>14497900000</v>
+        <v>1965975000</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
-        <v>2022</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>wake county board of education</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>school district of philadelphia</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Pennsylvania</t>
-        </is>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>13243.2734870299</v>
       </c>
       <c r="D10">
-        <v>29320.72882518869</v>
-      </c>
-      <c r="E10">
-        <v>3461400000</v>
+        <v>2120234842</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
-        <v>2022</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>dekalb county board of education</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>board of education of anne arundel county</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Maryland</t>
-        </is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>12116.3437784173</v>
       </c>
       <c r="D11">
-        <v>27584.88128133906</v>
-      </c>
-      <c r="E11">
-        <v>2294041482</v>
+        <v>1132551002</v>
       </c>
     </row>
   </sheetData>
@@ -1022,7 +952,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1031,238 +961,203 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>year</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>state.name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>state.name</t>
+          <t>total_pension_liability</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>total_pension_liability</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>total_pension_liability_pc</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>2022</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>hawaii department of education</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>rutherford county schools</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+          <t>Hawaii</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>city and county of denver school district no. 1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Colorado</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>30587841</v>
+      </c>
+      <c r="D3">
+        <v>344.027634375949</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>the school district of lee county</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>298857013</v>
+      </c>
+      <c r="D4">
+        <v>3072.637491774963</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>school district of polk county</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>299667822</v>
+      </c>
+      <c r="D5">
+        <v>2842.554893665459</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>duval county public schools</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>331630743</v>
+      </c>
+      <c r="D6">
+        <v>2571.817655178832</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>district school board of pinellas county</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>367120173</v>
+      </c>
+      <c r="D7">
+        <v>3846.365201265637</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>board of education of shelby county</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Tennessee</t>
         </is>
       </c>
-      <c r="D2">
-        <v>-76790573</v>
-      </c>
-      <c r="E2">
-        <v>-1559.104480945323</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2022</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>davis school district</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Utah</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>-65971070</v>
-      </c>
-      <c r="E3">
-        <v>-885.6841554117552</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>2022</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>granite school district</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Utah</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>-56371241</v>
-      </c>
-      <c r="E4">
-        <v>-901.3053370427219</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>2022</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>jordan school district</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Utah</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>-37798587</v>
-      </c>
-      <c r="E5">
-        <v>-636.7364688442295</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>2022</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>alpine school district</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Utah</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>-7711949</v>
-      </c>
-      <c r="E6">
-        <v>-89.38799188640974</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>2022</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>detroit public schools</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Michigan</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>2022</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>hawaii department of education</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Hawaii</t>
-        </is>
+      <c r="C8">
+        <v>402787448</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
+        <v>3814.419561347021</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>2022</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>northside independent school district (bexar county)</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>chesterfield county school board</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Virginia</t>
-        </is>
+          <t>Texas</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>425827219</v>
       </c>
       <c r="D9">
-        <v>4167372</v>
-      </c>
-      <c r="E9">
-        <v>66.73668027864521</v>
+        <v>4159.40317649472</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
-        <v>2022</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>cypress-fairbanks independent school district</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>city and county of denver school district no. 1</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Colorado</t>
-        </is>
+          <t>Texas</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>510161847</v>
       </c>
       <c r="D10">
-        <v>30587841</v>
-      </c>
-      <c r="E10">
-        <v>344.027634375949</v>
+        <v>4352.285479068736</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
-        <v>2022</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>orange county district school board</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>knox county schools</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Tennessee</t>
-        </is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>608004479</v>
       </c>
       <c r="D11">
-        <v>62560756</v>
-      </c>
-      <c r="E11">
-        <v>1035.328434779731</v>
+        <v>2991.794665000197</v>
       </c>
     </row>
   </sheetData>
@@ -1749,55 +1644,55 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>jacksonville</t>
+          <t>san jose</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>California</t>
         </is>
       </c>
       <c r="C9">
-        <v>3244209000</v>
+        <v>3116478000</v>
       </c>
       <c r="D9">
-        <v>3416.337761790029</v>
+        <v>3075.812680550443</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>san jose</t>
+          <t>fort worth</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C10">
-        <v>3116478000</v>
+        <v>2926444000</v>
       </c>
       <c r="D10">
-        <v>3075.812680550443</v>
+        <v>3184.596985429904</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>fort worth</t>
+          <t>san diego</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>California</t>
         </is>
       </c>
       <c r="C11">
-        <v>2926444000</v>
+        <v>2593890000</v>
       </c>
       <c r="D11">
-        <v>3184.596985429904</v>
+        <v>1870.198131164561</v>
       </c>
     </row>
   </sheetData>
@@ -1892,127 +1787,127 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>portland</t>
+          <t>worcester</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="C5">
-        <v>6714.114387649076</v>
+        <v>7338.302950333868</v>
       </c>
       <c r="D5">
-        <v>4381080492</v>
+        <v>1515498987</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>austin</t>
+          <t>portland</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="C6">
-        <v>6525.775028589251</v>
+        <v>6714.114387649076</v>
       </c>
       <c r="D6">
-        <v>6277143000</v>
+        <v>4381080492</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>rochester</t>
+          <t>austin</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>New York</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C7">
-        <v>5397.892306017859</v>
+        <v>6525.775028589251</v>
       </c>
       <c r="D7">
-        <v>1140688000</v>
+        <v>6277143000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>jersey city</t>
+          <t>rochester</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>New Jersey</t>
+          <t>New York</t>
         </is>
       </c>
       <c r="C8">
-        <v>5053.945097248885</v>
+        <v>5397.892306017859</v>
       </c>
       <c r="D8">
-        <v>1479562643</v>
+        <v>1140688000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>boston</t>
+          <t>jersey city</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="C9">
-        <v>5018.165214199445</v>
+        <v>5053.945097248885</v>
       </c>
       <c r="D9">
-        <v>3390433000</v>
+        <v>1479562643</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>buffalo</t>
+          <t>boston</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>New York</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="C10">
-        <v>4716.356930086489</v>
+        <v>5018.165214199445</v>
       </c>
       <c r="D10">
-        <v>1312566850</v>
+        <v>3390433000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>miami</t>
+          <t>buffalo</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>New York</t>
         </is>
       </c>
       <c r="C11">
-        <v>4700.251071767739</v>
+        <v>4716.356930086489</v>
       </c>
       <c r="D11">
-        <v>2078733039</v>
+        <v>1312566850</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding worcester total assets
</commit_message>
<xml_diff>
--- a/output/commentary_muni_debt_ranking.xlsx
+++ b/output/commentary_muni_debt_ranking.xlsx
@@ -1966,25 +1966,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>spokane</t>
+          <t>chula vista</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>California</t>
         </is>
       </c>
       <c r="C3">
-        <v>-196311784</v>
+        <v>-133323756</v>
       </c>
       <c r="D3">
-        <v>-857.3390631414371</v>
+        <v>-483.933778584392</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>chula vista</t>
+          <t>riverside</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1993,106 +1993,106 @@
         </is>
       </c>
       <c r="C4">
-        <v>-133323756</v>
+        <v>-91523000</v>
       </c>
       <c r="D4">
-        <v>-483.933778584392</v>
+        <v>-290.5362936250452</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>riverside</t>
+          <t>madison</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="C5">
-        <v>-91523000</v>
+        <v>-78290849</v>
       </c>
       <c r="D5">
-        <v>-290.5362936250452</v>
+        <v>-290.2144019512991</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>madison</t>
+          <t>plano</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C6">
-        <v>-78290849</v>
+        <v>-43321968</v>
       </c>
       <c r="D6">
-        <v>-290.2144019512991</v>
+        <v>-151.75717153176</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>plano</t>
+          <t>wichita</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C7">
-        <v>-43321968</v>
+        <v>-13760335</v>
       </c>
       <c r="D7">
-        <v>-151.75717153176</v>
+        <v>-34.61310235016237</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>wichita</t>
+          <t>santa clarita</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>California</t>
         </is>
       </c>
       <c r="C8">
-        <v>-13760335</v>
+        <v>-2504506</v>
       </c>
       <c r="D8">
-        <v>-34.61310235016237</v>
+        <v>-10.95205943702745</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>santa clarita</t>
+          <t>garland</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C9">
-        <v>-2504506</v>
+        <v>8188580</v>
       </c>
       <c r="D9">
-        <v>-10.95205943702745</v>
+        <v>33.28677525701115</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>garland</t>
+          <t>irving</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2101,28 +2101,28 @@
         </is>
       </c>
       <c r="C10">
-        <v>8188580</v>
+        <v>12758086</v>
       </c>
       <c r="D10">
-        <v>33.28677525701115</v>
+        <v>49.70289106966851</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>irving</t>
+          <t>aurora</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="C11">
-        <v>12758086</v>
+        <v>14138696</v>
       </c>
       <c r="D11">
-        <v>49.70289106966851</v>
+        <v>36.59802652695664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spokane 2022 opeb liabilities
</commit_message>
<xml_diff>
--- a/output/commentary_muni_debt_ranking.xlsx
+++ b/output/commentary_muni_debt_ranking.xlsx
@@ -1966,25 +1966,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>chula vista</t>
+          <t>spokane</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C3">
-        <v>-133323756</v>
+        <v>-196311784</v>
       </c>
       <c r="D3">
-        <v>-483.933778584392</v>
+        <v>-857.3390631414371</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>riverside</t>
+          <t>chula vista</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1993,106 +1993,106 @@
         </is>
       </c>
       <c r="C4">
-        <v>-91523000</v>
+        <v>-133323756</v>
       </c>
       <c r="D4">
-        <v>-290.5362936250452</v>
+        <v>-483.933778584392</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>madison</t>
+          <t>riverside</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>California</t>
         </is>
       </c>
       <c r="C5">
-        <v>-78290849</v>
+        <v>-91523000</v>
       </c>
       <c r="D5">
-        <v>-290.2144019512991</v>
+        <v>-290.5362936250452</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>plano</t>
+          <t>madison</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="C6">
-        <v>-43321968</v>
+        <v>-78290849</v>
       </c>
       <c r="D6">
-        <v>-151.75717153176</v>
+        <v>-290.2144019512991</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>wichita</t>
+          <t>plano</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C7">
-        <v>-13760335</v>
+        <v>-43321968</v>
       </c>
       <c r="D7">
-        <v>-34.61310235016237</v>
+        <v>-151.75717153176</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>santa clarita</t>
+          <t>wichita</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C8">
-        <v>-2504506</v>
+        <v>-13760335</v>
       </c>
       <c r="D8">
-        <v>-10.95205943702745</v>
+        <v>-34.61310235016237</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>garland</t>
+          <t>santa clarita</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>California</t>
         </is>
       </c>
       <c r="C9">
-        <v>8188580</v>
+        <v>-2504506</v>
       </c>
       <c r="D9">
-        <v>33.28677525701115</v>
+        <v>-10.95205943702745</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>irving</t>
+          <t>garland</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2101,28 +2101,28 @@
         </is>
       </c>
       <c r="C10">
-        <v>12758086</v>
+        <v>8188580</v>
       </c>
       <c r="D10">
-        <v>49.70289106966851</v>
+        <v>33.28677525701115</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>aurora</t>
+          <t>irving</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C11">
-        <v>14138696</v>
+        <v>12758086</v>
       </c>
       <c r="D11">
-        <v>36.59802652695664</v>
+        <v>49.70289106966851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>